<commit_message>
159 to 163 gomec andother added
</commit_message>
<xml_diff>
--- a/PPSPL PO NO 158.xlsx
+++ b/PPSPL PO NO 158.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prade\OneDrive\Desktop\pradeep_enterprises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEC0122-C5E5-4F8F-80D9-3445B44D131B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7CF69-927C-476C-AA8B-7138D9C69318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A3F91DE7-0C94-4712-A6AF-B1D21025C92A}"/>
   </bookViews>
@@ -372,42 +372,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,6 +421,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3789,166 +3789,166 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="33"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="33"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3957,37 +3957,37 @@
       <c r="H13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="17"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4">
         <v>4</v>
@@ -3995,21 +3995,21 @@
       <c r="H15" s="4">
         <v>2500</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="32">
         <v>10000</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4">
         <v>4</v>
@@ -4017,21 +4017,21 @@
       <c r="H16" s="4">
         <v>1500</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="32">
         <v>6000</v>
       </c>
-      <c r="J16" s="11"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4">
         <v>4</v>
@@ -4039,21 +4039,21 @@
       <c r="H17" s="4">
         <v>300</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="34">
         <v>1200</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>4</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
         <v>19</v>
@@ -4061,35 +4061,35 @@
       <c r="H18" s="4">
         <v>800</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="34">
         <v>3200</v>
       </c>
-      <c r="J18" s="11"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="11"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
         <v>4</v>
@@ -4097,258 +4097,258 @@
       <c r="H20" s="4">
         <v>550</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="32">
         <v>2200</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="11"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="11"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="11"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="11"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="11"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="11"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="34">
         <v>22600</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="33"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="32">
         <v>2034</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="32">
         <v>2034</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="11"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="33"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
       <c r="H33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="34">
         <v>26668</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="33"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
@@ -4357,42 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:E12"/>
-    <mergeCell ref="F5:J12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="I27:J27"/>
     <mergeCell ref="A34:J39"/>
     <mergeCell ref="A28:G33"/>
     <mergeCell ref="I28:J28"/>
@@ -4401,6 +4365,42 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:E12"/>
+    <mergeCell ref="F5:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>